<commit_message>
컬럼 삭제 * TBL_CONTROL_PART 	DETAIL_LATHE 	DETAIL_SURFACE 	DETAIL_CLAMPING 	DETAIL_POCKET 	DETAIL_DRILL 	DETAIL_DIFFICULTY 	UNIT_TM_AMT 	UNIT_GRIND_AMT 	UNIT_HEAT_AMT 	UNIT_MATERIAL_FINISH_AUTO_AMT 	UNIT_MATERIAL_FINISH_AMT 	UNIT_MATERIAL_AUTO_YN 	UNIT_TM_AUTO_YN 	UNIT_GRIND_AUTO_YN 	UNIT_HEAT_AUTO_YN 	UNIT_SURFACE_AUTO_YN 	UNIT_PROCESS_AUTO_YN
* TBL_ESTIMATE_DETAIL
	DETAIL_LATHE
	DETAIL_SURFACE
	DETAIL_CLAMPING
	DETAIL_POCKET
	DETAIL_DRILL
	DETAIL_DIFFICULTY
	UNIT_TM_AMT
	UNIT_GRIND_AMT
	UNIT_HEAT_AMT
	UNIT_MATERIAL_AUTO_YN
	UNIT_TM_AUTO_YN
	UNIT_GRIND_AUTO_YN
	UNIT_HEAT_AUTO_YN
	UNIT_SURFACE_AUTO_YN
</commit_message>
<xml_diff>
--- a/src/main/resources/excelTemplate/control_estimate_list_template.xlsx
+++ b/src/main/resources/excelTemplate/control_estimate_list_template.xlsx
@@ -238,14 +238,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${data.UNIT_TM_AMT}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>${data.UNIT_HEAT_AMT}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>${data.ROW_NUM}//:1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -291,6 +283,14 @@
   </si>
   <si>
     <t>${data.PREVIOUS_PRICE}//:1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${data.UNIT_MATERIAL_FINISH_TM_AMT}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${data.UNIT_MATERIAL_FINISH_HEAT_AMT}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -588,68 +588,68 @@
     <xf numFmtId="41" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="41" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="41" fontId="3" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1031,34 +1031,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="25" t="s">
         <v>27</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1067,16 +1067,16 @@
       <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="P1" s="23" t="s">
         <v>9</v>
       </c>
       <c r="Q1" s="3" t="s">
@@ -1088,50 +1088,50 @@
       <c r="S1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="T1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="V1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="W1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="X1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="29" t="s">
+      <c r="Y1" s="21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:25" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="16"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="26"/>
       <c r="K2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18" t="s">
+      <c r="M2" s="24"/>
+      <c r="N2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="18" t="s">
+      <c r="O2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="18" t="s">
+      <c r="P2" s="24" t="s">
         <v>32</v>
       </c>
       <c r="Q2" s="6" t="s">
@@ -1143,34 +1143,34 @@
       <c r="S2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="30"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="22"/>
     </row>
     <row r="3" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
-        <v>40</v>
+      <c r="A3" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="F3" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="G3" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>45</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>35</v>
@@ -1182,7 +1182,7 @@
         <v>37</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
@@ -1192,40 +1192,40 @@
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
-      <c r="T3" s="34" t="s">
+      <c r="T3" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="V3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="34" t="s">
+      <c r="W3" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="V3" s="25" t="s">
+      <c r="X3" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="W3" s="34" t="s">
+      <c r="Y3" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="X3" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y3" s="34" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="14" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
@@ -1235,22 +1235,24 @@
       <c r="Q4" s="9"/>
       <c r="R4" s="9"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="35"/>
-      <c r="X4" s="35"/>
-      <c r="Y4" s="35"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="Y1:Y2"/>
@@ -1267,15 +1269,13 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>